<commit_message>
ajustando trataticas e referencias
</commit_message>
<xml_diff>
--- a/data_input/base_cartorios_com_cns.xlsx
+++ b/data_input/base_cartorios_com_cns.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://documentalldoc-my.sharepoint.com/personal/igor_rocha_documentall_com_br/Documents/Documentall - ￃﾍgor/automacoes/carto.io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://documentalldoc-my.sharepoint.com/personal/igor_rocha_documentall_com_br/Documents/Documentos/igor-documentall/carto.io/data_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{7E2BB5D2-2D48-42B8-A1A9-73BFE2B9C774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54226605-3566-414D-A2C6-68A2D4639663}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{7E2BB5D2-2D48-42B8-A1A9-73BFE2B9C774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{047789BE-2282-4CB8-B2CC-6019A3264300}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4485" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="cns" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -11124,6 +11124,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -11141,20 +11155,6 @@
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -11169,7 +11169,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B4AEF0E-49F0-49CB-B75F-F4C4A9F82466}" name="tabela_cns" displayName="tabela_cns" ref="A1:A3680" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B4AEF0E-49F0-49CB-B75F-F4C4A9F82466}" name="tabela_cns" displayName="tabela_cns" ref="A1:A3680" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:A3680" xr:uid="{1B4AEF0E-49F0-49CB-B75F-F4C4A9F82466}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9F23864E-EB8E-4751-B599-905A66736798}" name="CNS"/>

</xml_diff>